<commit_message>
Adicionado alguns comentarios e opção para o usuário escolher o tema desejado do tranding.
</commit_message>
<xml_diff>
--- a/Trendings.xlsx
+++ b/Trendings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <x:si>
     <x:t>Trending</x:t>
   </x:si>
@@ -33,228 +33,243 @@
     <x:t>Tema</x:t>
   </x:si>
   <x:si>
+    <x:t>Mbappe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56,9 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Futebol · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ambev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10,1 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Assuntos do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jungkook</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,18 mi Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>K-pop · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Eduardo Girão</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.474 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Política · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senado Federal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21,1 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Assunto do Momento em Política</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>74,1 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pop · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Democracia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>153 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TAEKOOK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>132 mil Tweets</x:t>
+  </x:si>
+  <x:si>
     <x:t>Beyonce</x:t>
   </x:si>
   <x:si>
-    <x:t>217 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Assuntos do Momento</x:t>
+    <x:t>322 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#SamsungUnpacked</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71,9 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tecnologia · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Auckland City</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.195 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Câmara</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76,1 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Al Ahly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.429 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nikolas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46,2 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Galaxy S23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20,5 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#GalaxyUnpacked</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20,8 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fora Lula</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16,9 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cancelo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30,3 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.194 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tom Brady</x:t>
+  </x:si>
+  <x:si>
+    <x:t>207 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NFL · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marcel Van Hattem</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.279 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fenapaf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.859 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#CopaDaLigaNaESPN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MISS YOU ALBA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53,4 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Só no Twitter · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gisele</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,9 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Michael Jackson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56,2 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MITA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15,3 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rodrigo Pacheco</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45,9 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mundial de Clubes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9.913 Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Banrisul</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Campeonato Brasileiro · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fred Nicácio e Marília</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,1 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Assunto do Momento em Televisão</x:t>
   </x:si>
   <x:si>
     <x:t>lana</x:t>
   </x:si>
   <x:si>
-    <x:t>Pop · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#RENAISSANCEWorldTour</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16,5 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MITA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tom Brady</x:t>
-  </x:si>
-  <x:si>
-    <x:t>140 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NFL · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gisele</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9.066 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#REVERSA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comida · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Michael Jackson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>56,6 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rosa Weber</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.996 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Política · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Churrasco</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.610 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>João Rock</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unesp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.298 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#DemocraciaInabalada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3.141 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Câmara</x:t>
-  </x:si>
-  <x:si>
-    <x:t>63,6 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Florence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12,5 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Augusto Aras</x:t>
-  </x:si>
-  <x:si>
-    <x:t>61,9 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HOSEOK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>101 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>K-pop · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#democraciainabalada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.588 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patrícia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37,4 mil Tweets</x:t>
+    <x:t>116 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oscar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>447 mil Tweets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entretenimento · Assunto do Momento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dr fred</x:t>
+  </x:si>
+  <x:si>
+    <x:t>80 mil Tweets</x:t>
   </x:si>
   <x:si>
     <x:t>Programas de competição · Assunto do Momento</x:t>
   </x:si>
   <x:si>
-    <x:t>Publicitário</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.772 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Negócios &amp; finanças · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ozzy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13,2 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Música · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IPTV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6.157 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ana Clara</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.198 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Entretenimento · Assunto do Momento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Feijoada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.255 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>América do Norte</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.634 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Carol Biazin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.387 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>R$7,40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.053 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GOAT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>102 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Assembleia Legislativa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.590 Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fred Nicácio e Marília</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13,1 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Assunto do Momento em Televisão</x:t>
-  </x:si>
-  <x:si>
-    <x:t>116 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oscar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>447 mil Tweets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dr fred</x:t>
-  </x:si>
-  <x:si>
-    <x:t>80 mil Tweets</x:t>
-  </x:si>
-  <x:si>
     <x:t>Argentina</x:t>
   </x:si>
   <x:si>
@@ -286,9 +301,6 @@
   </x:si>
   <x:si>
     <x:t>BNDES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>76,1 mil Tweets</x:t>
   </x:si>
   <x:si>
     <x:t>BRILHA PRISCILA REIS</x:t>
@@ -718,7 +730,7 @@
       <x:selection activeCell="A1" sqref="A1"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="21.875781" defaultRowHeight="15.75" zeroHeight="false"/>
+  <x:sheetFormatPr defaultColWidth="23.297031" defaultRowHeight="15.75" zeroHeight="false"/>
   <x:cols>
     <x:col min="1" max="1" width="33.52" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="19.06" style="0" customWidth="1"/>
@@ -751,101 +763,107 @@
       <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A5" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A7" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A12" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>5</x:v>
@@ -853,208 +871,205 @@
     </x:row>
     <x:row r="13" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A13" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A14" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A15" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A16" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A17" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A18" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A19" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A20" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A21" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A22" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A23" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A24" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A25" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A26" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A27" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A28" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A29" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A30" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3" customFormat="1" ht="15.75" customHeight="1" outlineLevel="0">
       <x:c r="A31" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1081,7 +1096,7 @@
       <x:selection activeCell="A1" sqref="A1"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="17.207813" defaultRowHeight="15" zeroHeight="false"/>
+  <x:sheetFormatPr defaultColWidth="18.629063" defaultRowHeight="15" zeroHeight="false"/>
   <x:sheetData>
     <x:row r="1" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A1" s="0" t="s">
@@ -1096,156 +1111,156 @@
     </x:row>
     <x:row r="2" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A2" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A4" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A5" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A6" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A7" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A8" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A9" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A10" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A11" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A12" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A13" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A14" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A15" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>